<commit_message>
Manejo de alertas para algunos usuarios
</commit_message>
<xml_diff>
--- a/SQACompensar/Data/DatosCompensar.xlsx
+++ b/SQACompensar/Data/DatosCompensar.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28025"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAC26F24-5EDC-4A05-B004-2DEC2427460E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D4D45E1-FCA7-47B9-8DC6-646B459E2CE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -570,7 +570,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="B2" sqref="B2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -655,7 +655,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -691,7 +691,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1">
-        <v>53021207</v>
+        <v>1000005222</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>13</v>
@@ -703,7 +703,7 @@
         <v>8</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -711,7 +711,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="1">
-        <v>1000005222</v>
+        <v>53021207</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>13</v>
@@ -728,8 +728,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{28918E51-C663-430C-9DEA-E7ECD7D24868}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{133E747A-44DB-45A8-8789-732216D6459D}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{FA965B1F-6DCF-49F5-BAA7-BE35DE7D4ACF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -753,17 +753,17 @@
           </x14:formula1>
           <xm:sqref>A2:A3</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000004000000}">
-          <x14:formula1>
-            <xm:f>Listas!$N$2:$N$5</xm:f>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{701ED8FC-EC6C-4829-9157-9FA28D05CC5B}">
+          <x14:formula1>
+            <xm:f>Listas!$H$2:$H$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2:B3</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F1FA9FD1-1A0F-46B0-B911-17237450CBD5}">
+          <x14:formula1>
+            <xm:f>Listas!$I$2:$I$4</xm:f>
           </x14:formula1>
           <xm:sqref>C2:C3</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{65F150D7-12C3-4579-8550-9F8FBA3B7981}">
-          <x14:formula1>
-            <xm:f>Listas!$H$2:$H$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>B2:B3</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -860,7 +860,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -947,7 +947,7 @@
   <dimension ref="A1:O16"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -1046,7 +1046,7 @@
       <c r="F4" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="H4" s="1">
+      <c r="H4" s="14">
         <v>1000134386</v>
       </c>
       <c r="I4" t="s">

</xml_diff>